<commit_message>
HOBO Data first analysis
</commit_message>
<xml_diff>
--- a/URUVS/Datasheets/URUV/February/February_RecordingData.xlsx
+++ b/URUVS/Datasheets/URUV/February/February_RecordingData.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophi\Documents\GitHub\TanakekeProject\URUVS\Datasheets\February\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophi\Documents\GitHub\TanakekeProject\URUVS\Datasheets\URUV\February\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DD66F1F-E3B9-44D8-ADE2-E3EAF0506922}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C032890C-3662-41EA-AAE6-5AD637733E73}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="183">
   <si>
     <t>DATE</t>
   </si>
@@ -556,6 +556,30 @@
   </si>
   <si>
     <t>T1_UNIDGUPPY</t>
+  </si>
+  <si>
+    <t>LANTANGPEO</t>
+  </si>
+  <si>
+    <t>27_02_2024_1515_C1_D1_LTPE5</t>
+  </si>
+  <si>
+    <t>27_02_2024_1533_C5_D2_LTPE4</t>
+  </si>
+  <si>
+    <t>27_02_2024_1600_C11_D3_LTPL5</t>
+  </si>
+  <si>
+    <t>27_02_2024_1608_C12_D4_LTPD5</t>
+  </si>
+  <si>
+    <t>27_02_2024_1628_C14_D5_LTPL4</t>
+  </si>
+  <si>
+    <t>27_02_2024_1637_C15_D6_LTPD6</t>
+  </si>
+  <si>
+    <t>27_02_2024_1734_C1_D7_LTPE6</t>
   </si>
 </sst>
 </file>
@@ -2188,9 +2212,9 @@
   <dimension ref="A1:BT20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="4" topLeftCell="AL1" activePane="topRight" state="frozen"/>
+      <pane xSplit="4" topLeftCell="BB1" activePane="topRight" state="frozen"/>
       <selection activeCell="C1" sqref="C1"/>
-      <selection pane="topRight" activeCell="AS14" sqref="AS14"/>
+      <selection pane="topRight" activeCell="BM7" sqref="BM7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2424,7 +2448,7 @@
         <v>21</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>10</v>
+        <v>175</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>99</v>
@@ -2645,7 +2669,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>10</v>
+        <v>175</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>137</v>
@@ -2868,7 +2892,7 @@
         <v>25</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>10</v>
+        <v>175</v>
       </c>
       <c r="C4" s="9" t="s">
         <v>138</v>
@@ -2901,7 +2925,7 @@
         <v>50</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>28</v>
+        <v>176</v>
       </c>
       <c r="N4" s="9">
         <v>3</v>
@@ -3099,7 +3123,7 @@
         <v>25</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>10</v>
+        <v>175</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>138</v>
@@ -3132,7 +3156,7 @@
         <v>60</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>32</v>
+        <v>177</v>
       </c>
       <c r="N5" s="9">
         <v>2</v>
@@ -3322,7 +3346,7 @@
         <v>25</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>10</v>
+        <v>175</v>
       </c>
       <c r="C6" s="9" t="s">
         <v>137</v>
@@ -3355,7 +3379,7 @@
         <v>30</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>43</v>
+        <v>178</v>
       </c>
       <c r="N6" s="9">
         <v>3</v>
@@ -3547,7 +3571,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>10</v>
+        <v>175</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>99</v>
@@ -3580,7 +3604,7 @@
         <v>30</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>44</v>
+        <v>179</v>
       </c>
       <c r="N7" s="9">
         <v>3</v>
@@ -3772,7 +3796,7 @@
         <v>25</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>10</v>
+        <v>175</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>137</v>
@@ -3805,7 +3829,7 @@
         <v>40</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>45</v>
+        <v>180</v>
       </c>
       <c r="N8" s="9">
         <v>3</v>
@@ -3999,7 +4023,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>10</v>
+        <v>175</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>99</v>
@@ -4032,7 +4056,7 @@
         <v>35</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>46</v>
+        <v>181</v>
       </c>
       <c r="N9" s="9">
         <v>2</v>
@@ -4226,7 +4250,7 @@
         <v>25</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>10</v>
+        <v>175</v>
       </c>
       <c r="C10" s="9" t="s">
         <v>138</v>
@@ -4259,7 +4283,7 @@
         <v>39</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>47</v>
+        <v>182</v>
       </c>
       <c r="N10" s="9">
         <v>1</v>

</xml_diff>